<commit_message>
final cleaning of the time table
also some small changes in excel file temp_cleaned_finalversion
</commit_message>
<xml_diff>
--- a/_RESULTS/time_counts.xlsx
+++ b/_RESULTS/time_counts.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -400,7 +400,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>467</v>
+        <v>516</v>
       </c>
     </row>
     <row r="5">
@@ -410,157 +410,117 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>K2-Pg</t>
+          <t>Tr-J</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>171</v>
+        <v>338</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>J2</t>
+          <t>Pg</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>154</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Tr-J1</t>
+          <t>K2-Pg</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>122</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Tr3-J1</t>
+          <t>J2</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>121</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Pg</t>
+          <t>J1-J2</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>J1_2</t>
+          <t>Mz</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>109</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>K</t>
+          <t>J1</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>97</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Tr-J</t>
+          <t>K</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>95</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Mz</t>
+          <t>J</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>90</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Pg1</t>
+          <t>J-K</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>78</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>J1</t>
+          <t>J2-J3</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>J</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>J2_3</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>Tr3</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>Tr2</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
plotting time in qgis
</commit_message>
<xml_diff>
--- a/_RESULTS/time_counts.xlsx
+++ b/_RESULTS/time_counts.xlsx
@@ -390,7 +390,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1151</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="4">
@@ -400,7 +400,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="5">
@@ -430,7 +430,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8">
@@ -480,7 +480,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13">

</xml_diff>

<commit_message>
calculating the variance for each area
there are some samples without a time value, that's why there are more total samples than making the sum of each samples/area
-tried to do this in a for loop, but didn't work quite well, but the solution is also quite short
</commit_message>
<xml_diff>
--- a/_RESULTS/time_counts.xlsx
+++ b/_RESULTS/time_counts.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -376,21 +376,21 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>K2</t>
+          <t>K</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1271</v>
+        <v>2522</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>K1</t>
+          <t>J</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1152</v>
+        <v>825</v>
       </c>
     </row>
     <row r="4">
@@ -406,11 +406,11 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>J3</t>
+          <t>Pg</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>411</v>
+        <v>365</v>
       </c>
     </row>
     <row r="6">
@@ -426,101 +426,11 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Pg</t>
+          <t>Mz</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>K2-Pg</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>J2</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>J1-J2</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>Mz</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
         <v>88</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>J1</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>K</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>J</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>J-K</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>J2-J3</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>